<commit_message>
fixed bug now move to make weapon
</commit_message>
<xml_diff>
--- a/Mineral.xlsx
+++ b/Mineral.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -44,34 +44,13 @@
     <t>Showed Points</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
-    <t>testing</t>
-  </si>
-  <si>
-    <t>testing (3)</t>
-  </si>
-  <si>
-    <t>Sunstone</t>
-  </si>
-  <si>
-    <t>A radiant gem used for crafting luminous items.</t>
-  </si>
-  <si>
-    <t>Color [1,0.64705884,0,1]</t>
-  </si>
-  <si>
-    <t>(597,653);(577,276)</t>
-  </si>
-  <si>
-    <t>(597,653);(577,276);(596,652);(595,651);(594,650);(593,649);(592,648);(591,647);(590,646);(589,645);(588,644);(587,643);(586,642);(585,641);(584,640);(583,639);(582,638);(581,637);(580,636);(579,635);(578,634);(577,633);(577,632);(577,631);(577,630);(577,629);(577,628);(577,627);(577,626);(577,625);(577,624);(577,623);(577,622);(577,621);(577,620);(577,619);(577,618);(577,617);(577,616);(577,615);(577,614);(577,613);(577,612);(577,611);(577,610);(577,609);(577,608);(577,607);(577,606);(577,605);(577,604);(577,603);(577,602);(577,601);(577,600);(577,599);(577,598);(577,597);(577,596);(577,595);(577,594);(577,593);(577,592);(577,591);(577,590);(577,589);(577,588);(577,587);(577,586);(577,585);(577,584);(577,583);(577,582);(577,581);(577,580);(577,579);(577,578);(577,577);(577,576);(577,575);(577,574);(577,573);(577,572);(577,571);(577,570);(577,569);(577,568);(577,567);(577,566);(577,565);(577,564);(577,563);(577,562);(577,561);(577,560);(577,559);(577,558);(577,557);(577,556);(577,555);(577,554);(577,553);(577,552);(577,551);(577,550);(577,549);(577,548);(577,547);(577,546);(577,545);(577,544);(577,543);(577,542);(577,541);(577,540);(577,539);(577,538);(577,537);(577,536);(577,535);(577,534);(577,533);(577,532);(577,531);(577,530);(577,529);(577,528);(577,527);(577,526);(577,525);(577,524);(577,523);(577,522);(577,521);(577,520);(577,519);(577,518);(577,517);(577,516);(577,515);(577,514);(577,513);(577,512);(577,511);(577,510);(577,509);(577,508);(577,507);(577,506);(577,505);(577,504);(577,503);(577,502);(577,501);(577,500);(577,499);(577,498);(577,497);(577,496);(577,495);(577,494);(577,493);(577,492);(577,491);(577,490);(577,489);(577,488);(577,487);(577,486);(577,485);(577,484);(577,483);(577,482);(577,481);(577,480);(577,479);(577,478);(577,477);(577,476);(577,475);(577,474);(577,473);(577,472);(577,471);(577,470);(577,469);(577,468);(577,467);(577,466);(577,465);(577,464);(577,463);(577,462);(577,461);(577,460);(577,459);(577,458);(577,457);(577,456);(577,455);(577,454);(577,453);(577,452);(577,451);(577,450);(577,449);(577,448);(577,447);(577,446);(577,445);(577,444);(577,443);(577,442);(577,441);(577,440);(577,439);(577,438);(577,437);(577,436);(577,435);(577,434);(577,433);(577,432);(577,431);(577,430);(577,429);(577,428);(577,427);(577,426);(577,425);(577,424);(577,423);(577,422);(577,421);(577,420);(577,419);(577,418);(577,417);(577,416);(577,415);(577,414);(577,413);(577,412);(577,411);(577,410);(577,409);(577,408);(577,407);(577,406);(577,405);(577,404);(577,403);(577,402);(577,401);(577,400);(577,399);(577,398);(577,397);(577,396);(577,395);(577,394);(577,393);(577,392);(577,391);(577,390);(577,389);(577,388);(577,387);(577,386);(577,385);(577,384);(577,383);(577,382);(577,381);(577,380);(577,379);(577,378);(577,377);(577,376);(577,375);(577,374);(577,373);(577,372);(577,371);(577,370);(577,369);(577,368);(577,367);(577,366);(577,365);(577,364);(577,363);(577,362);(577,361);(577,360);(577,359);(577,358);(577,357);(577,356);(577,355);(577,354);(577,353);(577,352);(577,351);(577,350);(577,349);(577,348);(577,347);(577,346);(577,345);(577,344);(577,343);(577,342);(577,341);(577,340);(577,339);(577,338);(577,337);(577,336);(577,335);(577,334);(577,333);(577,332);(577,331);(577,330);(577,329);(577,328);(577,327);(577,326);(577,325);(577,324);(577,323);(577,322);(577,321);(577,320);(577,319);(577,318);(577,317);(577,316);(577,315);(577,314);(577,313);(577,312);(577,311);(577,310);(577,309);(577,308);(577,307);(577,306);(577,305);(577,304);(577,303);(577,302);(577,301);(577,300);(577,299);(577,298);(577,297);(577,296);(577,295);(577,294);(577,293);(577,292);(577,291);(577,290);(577,289);(577,288);(577,287);(577,286);(577,285);(577,284);(577,283);(577,282);(577,281);(577,280);(577,279);(577,278);(577,277);(577,276)</t>
-  </si>
-  <si>
-    <t>4</t>
-  </si>
-  <si>
-    <t>testing (4)</t>
+    <t>10</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t xml:space="preserve"> (10)</t>
   </si>
   <si>
     <t>Manganese</t>
@@ -83,106 +62,97 @@
     <t>Color [0.87058824,0.72156864,0.5294118,1]</t>
   </si>
   <si>
-    <t>(591,449);(706,359)</t>
-  </si>
-  <si>
-    <t>(591,449);(706,359);(592,448);(593,447);(594,446);(595,445);(596,444);(597,443);(598,442);(599,441);(600,440);(601,439);(602,438);(603,437);(604,436);(605,435);(606,434);(607,433);(608,432);(609,431);(610,430);(611,429);(612,428);(613,427);(614,426);(615,425);(616,424);(617,423);(618,422);(619,421);(620,420);(621,419);(622,418);(623,417);(624,416);(625,415);(626,414);(627,413);(628,412);(629,411);(630,410);(631,409);(632,408);(633,407);(634,406);(635,405);(636,404);(637,403);(638,402);(639,401);(640,400);(641,399);(642,398);(643,397);(644,396);(645,395);(646,394);(647,393);(648,392);(649,391);(650,390);(651,389);(652,388);(653,387);(654,386);(655,385);(656,384);(657,383);(658,382);(659,381);(660,380);(661,379);(662,378);(663,377);(664,376);(665,375);(666,374);(667,373);(668,372);(669,371);(670,370);(671,369);(672,368);(673,367);(674,366);(675,365);(676,364);(677,363);(678,362);(679,361);(680,360);(681,359);(682,359);(683,359);(684,359);(685,359);(686,359);(687,359);(688,359);(689,359);(690,359);(691,359);(692,359);(693,359);(694,359);(695,359);(696,359);(697,359);(698,359);(699,359);(700,359);(701,359);(702,359);(703,359);(704,359);(705,359);(706,359)</t>
+    <t>(549,602);(531,666)</t>
+  </si>
+  <si>
+    <t>(549,602);(531,666);(548,603);(547,604);(546,605);(545,606);(544,607);(543,608);(542,609);(541,610);(540,611);(539,612);(538,613);(537,614);(536,615);(535,616);(534,617);(533,618);(532,619);(531,620);(531,621);(531,622);(531,623);(531,624);(531,625);(531,626);(531,627);(531,628);(531,629);(531,630);(531,631);(531,632);(531,633);(531,634);(531,635);(531,636);(531,637);(531,638);(531,639);(531,640);(531,641);(531,642);(531,643);(531,644);(531,645);(531,646);(531,647);(531,648);(531,649);(531,650);(531,651);(531,652);(531,653);(531,654);(531,655);(531,656);(531,657);(531,658);(531,659);(531,660);(531,661);(531,662);(531,663);(531,664);(531,665);(531,666)</t>
+  </si>
+  <si>
+    <t>(247,478);(477,720)</t>
+  </si>
+  <si>
+    <t>(247,478);(477,720);(248,479);(249,480);(250,481);(251,482);(252,483);(253,484);(254,485);(255,486);(256,487);(257,488);(258,489);(259,490);(260,491);(261,492);(262,493);(263,494);(264,495);(265,496);(266,497);(267,498);(268,499);(269,500);(270,501);(271,502);(272,503);(273,504);(274,505);(275,506);(276,507);(277,508);(278,509);(279,510);(280,511);(281,512);(282,513);(283,514);(284,515);(285,516);(286,517);(287,518);(288,519);(289,520);(290,521);(291,522);(292,523);(293,524);(294,525);(295,526);(296,527);(297,528);(298,529);(299,530);(300,531);(301,532);(302,533);(303,534);(304,535);(305,536);(306,537);(307,538);(308,539);(309,540);(310,541);(311,542);(312,543);(313,544);(314,545);(315,546);(316,547);(317,548);(318,549);(319,550);(320,551);(321,552);(322,553);(323,554);(324,555);(325,556);(326,557);(327,558);(328,559);(329,560);(330,561);(331,562);(332,563);(333,564);(334,565);(335,566);(336,567);(337,568);(338,569);(339,570);(340,571);(341,572);(342,573);(343,574);(344,575);(345,576);(346,577);(347,578);(348,579);(349,580);(350,581);(351,582);(352,583);(353,584);(354,585);(355,586);(356,587);(357,588);(358,589);(359,590);(360,591);(361,592);(362,593);(363,594);(364,595);(365,596);(366,597);(367,598);(368,599);(369,600);(370,601);(371,602);(372,603);(373,604);(374,605);(375,606);(376,607);(377,608);(378,609);(379,610);(380,611);(381,612);(382,613);(383,614);(384,615);(385,616);(386,617);(387,618);(388,619);(389,620);(390,621);(391,622);(392,623);(393,624);(394,625);(395,626);(396,627);(397,628);(398,629);(399,630);(400,631);(401,632);(402,633);(403,634);(404,635);(405,636);(406,637);(407,638);(408,639);(409,640);(410,641);(411,642);(412,643);(413,644);(414,645);(415,646);(416,647);(417,648);(418,649);(419,650);(420,651);(421,652);(422,653);(423,654);(424,655);(425,656);(426,657);(427,658);(428,659);(429,660);(430,661);(431,662);(432,663);(433,664);(434,665);(435,666);(436,667);(437,668);(438,669);(439,670);(440,671);(441,672);(442,673);(443,674);(444,675);(445,676);(446,677);(447,678);(448,679);(449,680);(450,681);(451,682);(452,683);(453,684);(454,685);(455,686);(456,687);(457,688);(458,689);(459,690);(460,691);(461,692);(462,693);(463,694);(464,695);(465,696);(466,697);(467,698);(468,699)</t>
+  </si>
+  <si>
+    <t>(618,546);(466,261)</t>
+  </si>
+  <si>
+    <t>(618,546);(466,261);(617,545);(616,544);(615,543);(614,542);(613,541);(612,540);(611,539);(610,538);(609,537);(608,536);(607,535);(606,534);(605,533);(604,532);(603,531);(602,530);(601,529);(600,528);(599,527);(598,526);(597,525);(596,524);(595,523);(594,522);(593,521);(592,520);(591,519);(590,518);(589,517);(588,516);(587,515);(586,514);(585,513);(584,512);(583,511);(582,510);(581,509);(580,508);(579,507);(578,506);(577,505);(576,504);(575,503);(574,502);(573,501);(572,500);(571,499);(570,498);(569,497);(568,496);(567,495);(566,494);(565,493);(564,492);(563,491);(562,490);(561,489);(560,488);(559,487);(558,486);(557,485);(556,484);(555,483);(554,482);(553,481);(552,480);(551,479);(550,478);(549,477);(548,476);(547,475);(546,474);(545,473);(544,472);(543,471);(542,470);(541,469);(540,468);(539,467);(538,466);(537,465);(536,464);(535,463);(534,462);(533,461);(532,460);(531,459);(530,458);(529,457);(528,456);(527,455);(526,454);(525,453);(524,452);(523,451);(522,450);(521,449);(520,448);(519,447);(518,446);(517,445);(516,444);(515,443);(514,442);(513,441);(512,440);(511,439);(510,438);(509,437);(508,436);(507,435);(506,434);(505,433);(504,432);(503,431);(502,430);(501,429);(500,428);(499,427);(498,426);(497,425);(496,424);(495,423);(494,422);(493,421);(492,420);(491,419);(490,418);(489,417);(488,416);(487,415);(486,414);(485,413);(484,412);(483,411);(482,410);(481,409);(480,408);(479,407);(478,406);(477,405);(476,404);(475,403);(474,402);(473,401);(472,400);(471,399);(470,398);(469,397);(468,396);(467,395);(466,394);(466,393);(466,392);(466,391);(466,390);(466,389);(466,388);(466,387);(466,386);(466,385);(466,384);(466,383);(466,382);(466,381);(466,380);(466,379);(466,378);(466,377);(466,376);(466,375);(466,374);(466,373);(466,372);(466,371);(466,370);(466,369);(466,368);(466,367);(466,366);(466,365);(466,364);(466,363);(466,362);(466,361);(466,360);(466,359);(466,358);(466,357);(466,356);(466,355);(466,354);(466,353);(466,352);(466,351);(466,350);(466,349);(466,348);(466,347);(466,346);(466,345);(466,344);(466,343);(466,342);(466,341);(466,340);(466,339);(466,338);(466,337);(466,336);(466,335);(466,334);(466,333);(466,332);(466,331);(466,330);(466,329);(466,328);(466,327);(466,326);(466,325);(466,324);(466,323);(466,322);(466,321);(466,320);(466,319);(466,318);(466,317);(466,316);(466,315);(466,314);(466,313);(466,312);(466,311);(466,310);(466,309);(466,308);(466,307);(466,306);(466,305);(466,304);(466,303);(466,302);(466,301);(466,300);(466,299);(466,298);(466,297);(466,296);(466,295);(466,294);(466,293);(466,292);(466,291);(466,290);(466,289);(466,288);(466,287);(466,286);(466,285);(466,284);(466,283);(466,282);(466,281);(466,280);(466,279);(466,278);(466,277);(466,276);(466,275);(466,274);(466,273);(466,272);(466,271);(466,270);(466,269);(466,268);(466,267);(466,266);(466,265);(466,264);(466,263);(466,262);(466,261)</t>
+  </si>
+  <si>
+    <t>Silver Ore</t>
+  </si>
+  <si>
+    <t>A precious metal used for crafting jewelry and decorative items.</t>
+  </si>
+  <si>
+    <t>Color [0.7529412,0.7529412,0.7529412,1]</t>
+  </si>
+  <si>
+    <t>(728,390);(720,252)</t>
+  </si>
+  <si>
+    <t>(728,390);(720,252);(727,389);(726,388);(725,387);(724,386);(723,385);(722,384);(721,383);(720,382);(720,381);(720,380);(720,379);(720,378);(720,377);(720,376);(720,375);(720,374);(720,373);(720,372);(720,371);(720,370);(720,369);(720,368);(720,367);(720,366);(720,365);(720,364);(720,363);(720,362);(720,361);(720,360);(720,359);(720,358);(720,357);(720,356);(720,355);(720,354);(720,353);(720,352);(720,351);(720,350);(720,349);(720,348);(720,347);(720,346);(720,345);(720,344);(720,343);(720,342);(720,341);(720,340);(720,339);(720,338);(720,337);(720,336);(720,335);(720,334);(720,333);(720,332);(720,331);(720,330);(720,329);(720,328);(720,327);(720,326);(720,325);(720,324);(720,323);(720,322);(720,321);(720,320);(720,319);(720,318);(720,317);(720,316);(720,315);(720,314);(720,313);(720,312);(720,311);(720,310);(720,309);(720,308);(720,307);(720,306);(720,305);(720,304);(720,303);(720,302);(720,301);(720,300);(720,299);(720,298);(720,297);(720,296);(720,295);(720,294);(720,293);(720,292);(720,291);(720,290);(720,289);(720,288);(720,287);(720,286);(720,285);(720,284);(720,283);(720,282);(720,281);(720,280);(720,279);(720,278);(720,277);(720,276);(720,275);(720,274);(720,273);(720,272);(720,271);(720,270);(720,269);(720,268);(720,267);(720,266);(720,265);(720,264);(720,263);(720,262);(720,261);(720,260);(720,259);(720,258);(720,257);(720,256);(720,255);(720,254);(720,253);(720,252)</t>
   </si>
   <si>
     <t>5</t>
   </si>
   <si>
-    <t>testing (5)</t>
-  </si>
-  <si>
-    <t>(360,344);(736,472)</t>
-  </si>
-  <si>
-    <t>(360,344);(736,472);(361,345);(362,346);(363,347);(364,348);(365,349);(366,350);(367,351);(368,352);(369,353);(370,354);(371,355);(372,356);(373,357);(374,358);(375,359);(376,360);(377,361);(378,362);(379,363);(380,364);(381,365);(382,366);(383,367);(384,368);(385,369);(386,370);(387,371);(388,372);(389,373);(390,374);(391,375);(392,376);(393,377);(394,378);(395,379);(396,380);(397,381);(398,382);(399,383);(400,384);(401,385);(402,386);(403,387);(404,388);(405,389);(406,390);(407,391);(408,392);(409,393);(410,394);(411,395);(412,396);(413,397);(414,398);(415,399);(416,400);(417,401);(418,402);(419,403);(420,404);(421,405);(422,406);(423,407);(424,408);(425,409);(426,410);(427,411);(428,412);(429,413);(430,414);(431,415);(432,416);(433,417);(434,418);(435,419);(436,420);(437,421);(438,422);(439,423);(440,424);(441,425);(442,426);(443,427);(444,428);(445,429);(446,430);(447,431);(448,432);(449,433);(450,434);(451,435);(452,436);(453,437);(454,438);(455,439);(456,440);(457,441);(458,442);(459,443);(460,444);(461,445);(462,446);(463,447);(464,448);(465,449);(466,450);(467,451);(468,452);(469,453);(470,454);(471,455);(472,456);(473,457);(474,458);(475,459);(476,460);(477,461);(478,462);(479,463);(480,464);(481,465);(482,466);(483,467);(484,468);(485,469);(486,470);(487,471);(488,472);(489,472);(490,472);(491,472);(492,472);(493,472);(494,472);(495,472);(496,472);(497,472);(498,472);(499,472);(500,472);(501,472);(502,472);(503,472);(504,472);(505,472);(506,472);(507,472);(508,472);(509,472);(510,472);(511,472);(512,472);(513,472);(514,472);(515,472);(516,472);(517,472);(518,472);(519,472);(520,472);(521,472);(522,472);(523,472);(524,472);(525,472);(526,472);(527,472);(528,472);(529,472);(530,472);(531,472);(532,472);(533,472);(534,472);(535,472);(536,472);(537,472);(538,472);(539,472);(540,472);(541,472);(542,472);(543,472);(544,472);(545,472);(546,472);(547,472);(548,472);(549,472);(550,472);(551,472);(552,472);(553,472);(554,472);(555,472);(556,472);(557,472);(558,472);(559,472);(560,472);(561,472);(562,472);(563,472);(564,472);(565,472);(566,472);(567,472);(568,472);(569,472);(570,472);(571,472);(572,472);(573,472);(574,472);(575,472);(576,472);(577,472);(578,472);(579,472);(580,472);(581,472);(582,472);(583,472);(584,472);(585,472);(586,472);(587,472);(588,472);(589,472);(590,472);(591,472);(592,472);(593,472);(594,472);(595,472);(596,472);(597,472);(598,472);(599,472);(600,472);(601,472);(602,472);(603,472);(604,472);(605,472);(606,472);(607,472);(608,472);(609,472);(610,472);(611,472);(612,472);(613,472);(614,472);(615,472);(616,472);(617,472);(618,472);(619,472);(620,472);(621,472);(622,472);(623,472);(624,472);(625,472);(626,472);(627,472);(628,472);(629,472);(630,472);(631,472);(632,472);(633,472);(634,472);(635,472);(636,472);(637,472);(638,472);(639,472);(640,472);(641,472);(642,472);(643,472);(644,472);(645,472);(646,472);(647,472);(648,472);(649,472);(650,472);(651,472);(652,472);(653,472);(654,472);(655,472);(656,472);(657,472);(658,472);(659,472);(660,472);(661,472);(662,472);(663,472);(664,472);(665,472);(666,472);(667,472);(668,472);(669,472);(670,472);(671,472);(672,472);(673,472);(674,472);(675,472);(676,472);(677,472);(678,472);(679,472);(680,472);(681,472);(682,472);(683,472);(684,472);(685,472);(686,472);(687,472);(688,472);(689,472);(690,472);(691,472);(692,472);(693,472);(694,472);(695,472);(696,472);(697,472);(698,472);(699,472);(700,472);(701,472);(702,472);(703,472);(704,472);(705,472);(706,472);(707,472);(708,472);(709,472);(710,472);(711,472);(712,472);(713,472);(714,472);(715,472);(716,472);(717,472);(718,472);(719,472);(720,472);(721,472);(722,472);(723,472);(724,472);(725,472);(726,472);(727,472);(728,472);(729,472);(730,472);(731,472);(732,472);(733,472);(734,472);(735,472);(736,472)</t>
+    <t xml:space="preserve"> (5)</t>
+  </si>
+  <si>
+    <t>(401,594);(348,696)</t>
+  </si>
+  <si>
+    <t>(401,594);(348,696);(400,595);(399,596);(398,597);(397,598);(396,599);(395,600);(394,601);(393,602);(392,603);(391,604);(390,605);(389,606);(388,607);(387,608);(386,609);(385,610);(384,611);(383,612);(382,613);(381,614);(380,615);(379,616);(378,617);(377,618);(376,619);(375,620);(374,621);(373,622);(372,623);(371,624);(370,625);(369,626);(368,627);(367,628);(366,629);(365,630);(364,631);(363,632);(362,633);(361,634);(360,635);(359,636);(358,637);(357,638);(356,639);(355,640);(354,641);(353,642);(352,643);(351,644);(350,645);(349,646);(348,647);(348,648);(348,649);(348,650);(348,651);(348,652);(348,653);(348,654);(348,655);(348,656);(348,657);(348,658);(348,659);(348,660);(348,661);(348,662);(348,663);(348,664);(348,665);(348,666);(348,667);(348,668);(348,669);(348,670);(348,671);(348,672);(348,673);(348,674);(348,675);(348,676);(348,677);(348,678);(348,679);(348,680);(348,681);(348,682);(348,683);(348,684);(348,685);(348,686);(348,687);(348,688);(348,689);(348,690);(348,691);(348,692);(348,693);(348,694);(348,695);(348,696);(345,457)</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (6)</t>
+  </si>
+  <si>
+    <t>(263,433);(249,561)</t>
+  </si>
+  <si>
+    <t>(263,433);(249,561);(262,434);(261,435);(260,436);(259,437);(258,438);(257,439);(256,440);(255,441);(254,442);(253,443);(252,444);(251,445);(250,446);(249,447);(249,448);(249,449);(249,450);(249,451);(249,452);(249,453);(249,454);(249,455);(249,456);(249,457);(249,458);(249,459);(249,460);(249,461);(249,462);(249,463);(249,464);(249,465);(249,466);(249,467);(249,468);(249,469);(249,470);(249,471);(249,472);(249,473);(249,474);(249,475);(249,476);(249,477);(249,478);(249,479);(249,480);(249,481);(249,482);(249,483);(249,484);(249,485);(249,486);(249,487);(249,488);(249,489);(249,490);(249,491);(249,492);(249,493);(249,494);(249,495);(249,496);(249,497);(249,498);(249,499);(249,500);(249,501);(249,502);(249,503);(249,504);(249,505);(249,506);(249,507);(249,508);(249,509);(249,510);(249,511);(249,512);(249,513);(249,514);(249,515);(249,516);(249,517);(249,518);(249,519);(249,520);(249,521);(249,522);(249,523);(249,524);(249,525);(249,526);(249,527);(249,528);(249,529);(249,530);(249,531);(249,532);(249,533);(249,534);(249,535);(249,536);(249,537);(249,538);(249,539);(249,540);(249,541);(249,542);(249,543);(249,544);(249,545);(249,546);(249,547);(249,548);(249,549);(249,550);(249,551);(249,552);(249,553);(249,554);(249,555);(249,556);(249,557);(249,558);(249,559);(249,560);(249,561)</t>
   </si>
   <si>
     <t>7</t>
   </si>
   <si>
-    <t>testing (7)</t>
-  </si>
-  <si>
-    <t>(635,251);(282,650)</t>
-  </si>
-  <si>
-    <t>(635,251);(282,650);(634,252);(633,253);(632,254);(631,255);(630,256);(629,257);(628,258);(627,259);(626,260);(625,261);(624,262);(623,263);(622,264);(621,265);(620,266);(619,267);(618,268);(617,269);(616,270);(615,271);(614,272);(613,273);(612,274);(611,275);(610,276);(609,277);(608,278);(607,279);(606,280);(605,281);(604,282);(603,283);(602,284);(601,285);(600,286);(599,287);(598,288);(597,289);(596,290);(595,291);(594,292);(593,293);(592,294);(591,295);(590,296);(589,297);(588,298);(587,299);(586,300);(585,301);(584,302);(583,303);(582,304);(581,305);(580,306);(579,307);(578,308);(577,309);(576,310);(575,311);(574,312);(573,313);(572,314);(571,315);(570,316);(569,317);(568,318);(567,319);(566,320);(565,321);(564,322);(563,323);(562,324);(561,325);(560,326);(559,327);(558,328);(557,329);(556,330);(555,331);(554,332);(553,333);(552,334);(551,335);(550,336);(549,337);(548,338);(547,339);(546,340);(545,341);(544,342);(543,343);(542,344);(541,345);(540,346);(539,347);(538,348);(537,349);(536,350);(535,351);(534,352);(533,353);(532,354);(531,355);(530,356);(529,357);(528,358);(527,359);(526,360);(525,361);(524,362);(523,363);(522,364);(521,365);(520,366);(519,367);(518,368);(517,369);(516,370);(515,371);(514,372);(513,373);(512,374);(511,375);(510,376);(509,377);(508,378);(507,379);(506,380);(505,381);(504,382);(503,383);(502,384);(501,385);(500,386);(499,387);(498,388);(497,389);(496,390);(495,391);(494,392);(493,393);(492,394);(491,395);(490,396);(489,397);(488,398);(487,399);(486,400);(485,401);(484,402);(483,403);(482,404);(481,405);(480,406);(479,407);(478,408);(477,409);(476,410);(475,411);(474,412);(473,413);(472,414);(471,415);(470,416);(469,417);(468,418);(467,419);(466,420);(465,421);(464,422);(463,423);(462,424);(461,425);(460,426);(459,427);(458,428);(457,429);(456,430);(455,431);(454,432);(453,433);(452,434);(451,435);(450,436);(449,437);(448,438);(447,439);(446,440);(445,441);(444,442);(443,443);(442,444);(441,445);(440,446);(439,447);(438,448);(437,449);(436,450);(435,451);(434,452);(433,453);(432,454);(431,455);(430,456);(429,457);(428,458);(427,459);(426,460);(425,461);(424,462);(423,463);(422,464);(421,465);(420,466);(419,467);(418,468);(417,469);(416,470);(415,471);(414,472);(413,473);(412,474);(411,475);(410,476);(409,477);(408,478);(407,479);(406,480);(405,481);(404,482);(403,483);(402,484);(401,485);(400,486);(399,487);(398,488);(397,489);(396,490);(395,491);(394,492);(393,493);(392,494);(391,495);(390,496);(389,497);(388,498);(387,499);(386,500);(385,501);(384,502);(383,503);(382,504);(381,505);(380,506);(379,507);(378,508);(377,509);(376,510);(375,511);(374,512);(373,513);(372,514);(371,515);(370,516);(369,517);(368,518);(367,519);(366,520);(365,521);(364,522);(363,523);(362,524);(361,525);(360,526);(359,527);(358,528);(357,529);(356,530);(355,531);(354,532);(353,533);(352,534);(351,535);(350,536);(349,537);(348,538);(347,539);(346,540);(345,541);(344,542);(343,543);(342,544);(341,545);(340,546);(339,547);(338,548);(337,549);(336,550);(335,551);(334,552);(333,553);(332,554);(331,555);(330,556);(329,557);(328,558);(327,559);(326,560);(325,561);(324,562);(323,563);(322,564);(321,565);(320,566);(319,567);(318,568);(317,569);(316,570);(315,571);(314,572);(313,573);(312,574);(311,575);(310,576);(309,577);(308,578);(307,579);(306,580);(305,581);(304,582);(303,583);(302,584);(301,585);(300,586);(299,587);(298,588);(297,589);(296,590);(295,591);(294,592);(293,593);(292,594);(291,595);(290,596);(289,597);(288,598);(287,599);(286,600);(285,601);(284,602);(283,603);(282,604);(282,605);(282,606);(282,607);(282,608);(282,609);(282,610);(282,611);(282,612);(282,613);(282,614);(282,615);(282,616);(282,617);(282,618);(282,619);(282,620);(282,621);(282,622);(282,623);(282,624);(282,625);(282,626);(282,627);(282,628);(282,629);(282,630);(282,631);(282,632);(282,633);(282,634);(282,635);(282,636);(282,637);(282,638);(282,639);(282,640);(282,641);(282,642);(282,643);(282,644);(282,645);(282,646);(282,647);(282,648);(282,649);(282,650)</t>
+    <t xml:space="preserve"> (7)</t>
+  </si>
+  <si>
+    <t>(532,289);(241,251)</t>
+  </si>
+  <si>
+    <t>(532,289);(241,251);(531,288);(530,287);(529,286);(528,285);(527,284);(526,283);(525,282);(524,281);(523,280);(522,279);(521,278);(520,277);(519,276);(518,275);(517,274);(516,273);(515,272);(514,271);(513,270);(512,269);(511,268);(510,267);(509,266);(508,265);(507,264);(506,263);(505,262);(504,261);(503,260);(502,259);(501,258);(500,257);(499,256);(498,255);(497,254);(496,253);(495,252);(494,251);(493,251);(492,251);(491,251);(490,251);(489,251);(488,251);(487,251);(486,251);(485,251);(484,251);(483,251);(482,251);(481,251);(480,251);(479,251);(478,251);(477,251);(476,251);(475,251);(474,251);(473,251);(472,251);(471,251);(470,251);(469,251);(468,251);(467,251);(466,251);(465,251);(464,251);(463,251);(462,251);(461,251);(460,251);(459,251);(458,251);(457,251);(456,251);(455,251);(454,251);(453,251);(452,251);(451,251);(450,251);(449,251);(448,251);(447,251);(446,251);(445,251);(444,251);(443,251);(442,251);(441,251);(440,251);(439,251);(438,251);(437,251);(436,251);(435,251);(434,251);(433,251);(432,251);(431,251);(430,251);(429,251);(428,251);(427,251);(426,251);(425,251);(424,251);(423,251);(422,251);(421,251);(420,251);(419,251);(418,251);(417,251);(416,251);(415,251);(414,251);(413,251);(412,251);(411,251);(410,251);(409,251);(408,251);(407,251);(406,251);(405,251);(404,251);(403,251);(402,251);(401,251);(400,251);(399,251);(398,251);(397,251);(396,251);(395,251);(394,251);(393,251);(392,251);(391,251);(390,251);(389,251);(388,251);(387,251);(386,251);(385,251);(384,251);(383,251);(382,251);(381,251);(380,251);(379,251);(378,251);(377,251);(376,251);(375,251);(374,251);(373,251);(372,251);(371,251);(370,251);(369,251);(368,251);(367,251);(366,251);(365,251);(364,251);(363,251);(362,251);(361,251);(360,251);(359,251);(358,251);(357,251);(356,251);(355,251);(354,251);(353,251);(352,251);(351,251);(350,251);(349,251);(348,251);(347,251);(346,251);(345,251);(344,251);(343,251);(342,251);(341,251);(340,251);(339,251);(338,251);(337,251);(336,251);(335,251);(334,251);(333,251);(332,251);(331,251);(330,251);(329,251);(328,251);(327,251);(326,251);(325,251);(324,251);(323,251);(322,251);(321,251);(320,251);(319,251);(318,251);(317,251);(316,251);(315,251);(314,251);(313,251);(312,251);(311,251);(310,251);(309,251);(308,251);(307,251);(306,251);(305,251);(304,251);(303,251);(302,251);(301,251);(300,251);(299,251);(298,251);(297,251);(296,251);(295,251);(294,251);(293,251);(292,251);(291,251);(290,251);(289,251);(288,251);(287,251);(286,251);(285,251);(284,251);(283,251);(282,251);(281,251);(280,251);(279,251);(278,251);(277,251);(276,251);(275,251);(274,251);(273,251);(272,251);(271,251);(270,251);(269,251);(268,251);(267,251);(266,251);(265,251);(264,251);(263,251);(262,251);(261,251);(260,251);(259,251);(258,251);(257,251);(256,251);(255,251);(254,251);(253,251);(252,251);(251,251);(250,251);(249,251);(248,251);(247,251);(246,251);(245,251);(244,251);(243,251);(242,251);(241,251)</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t>testing (8)</t>
-  </si>
-  <si>
-    <t>(742,589);(419,307)</t>
-  </si>
-  <si>
-    <t>(742,589);(419,307);(741,588);(740,587);(739,586);(738,585);(737,584);(736,583);(735,582);(734,581);(733,580);(732,579);(731,578);(730,577);(729,576);(728,575);(727,574);(726,573);(725,572);(724,571);(723,570);(722,569);(721,568);(720,567);(719,566);(718,565);(717,564);(716,563);(715,562);(714,561);(713,560);(712,559);(711,558);(710,557);(709,556);(708,555);(707,554);(706,553);(705,552);(704,551);(703,550);(702,549);(701,548);(700,547);(699,546);(698,545);(697,544);(696,543);(695,542);(694,541);(693,540);(692,539);(691,538);(690,537);(689,536);(688,535);(687,534);(686,533);(685,532);(684,531);(683,530);(682,529);(681,528);(680,527);(679,526);(678,525);(677,524);(676,523);(675,522);(674,521);(673,520);(672,519);(671,518);(670,517);(669,516);(668,515);(667,514);(666,513);(665,512);(664,511);(663,510);(662,509);(661,508);(660,507);(659,506);(658,505);(657,504);(656,503);(655,502);(654,501);(653,500);(652,499);(651,498);(650,497);(649,496);(648,495);(647,494);(646,493);(645,492);(644,491);(643,490);(642,489);(641,488);(640,487);(639,486);(638,485);(637,484);(636,483);(635,482);(634,481);(633,480);(632,479);(631,478);(630,477);(629,476);(628,475);(627,474);(626,473);(625,472);(624,471);(623,470);(622,469);(621,468);(620,467);(619,466);(618,465);(617,464);(616,463);(615,462);(614,461);(613,460);(612,459);(611,458);(610,457);(609,456);(608,455);(607,454);(606,453);(605,452);(604,451);(603,450);(602,449);(601,448);(600,447);(599,446);(598,445);(597,444);(596,443);(595,442);(594,441);(593,440);(592,439);(591,438);(590,437);(589,436);(588,435);(587,434);(586,433);(585,432);(584,431);(583,430);(582,429);(581,428);(580,427);(579,426);(578,425);(577,424);(576,423);(575,422);(574,421);(573,420);(572,419);(571,418);(570,417);(569,416);(568,415);(567,414);(566,413);(565,412);(564,411);(563,410);(562,409);(561,408);(560,407);(559,406);(558,405);(557,404);(556,403);(555,402);(554,401);(553,400);(552,399);(551,398);(550,397);(549,396);(548,395);(547,394);(546,393);(545,392);(544,391);(543,390);(542,389);(541,388);(540,387);(539,386);(538,385);(537,384);(536,383);(535,382);(534,381);(533,380);(532,379);(531,378);(530,377);(529,376);(528,375);(527,374);(526,373);(525,372);(524,371);(523,370);(522,369);(521,368);(520,367);(519,366);(518,365);(517,364);(516,363);(515,362);(514,361);(513,360);(512,359);(511,358);(510,357);(509,356);(508,355);(507,354);(506,353);(505,352);(504,351);(503,350);(502,349);(501,348);(500,347);(499,346);(498,345);(497,344);(496,343);(495,342);(494,341);(493,340);(492,339);(491,338);(490,337);(489,336);(488,335);(487,334);(486,333);(485,332);(484,331);(483,330);(482,329);(481,328);(480,327);(479,326);(478,325);(477,324);(476,323);(475,322);(474,321);(473,320);(472,319);(471,318);(470,317);(469,316);(468,315);(467,314);(466,313);(465,312);(464,311);(463,310);(462,309);(461,308);(460,307);(459,307);(458,307);(457,307);(456,307);(455,307);(454,307);(453,307);(452,307);(451,307);(450,307);(449,307);(448,307);(447,307);(446,307);(445,307);(444,307);(443,307);(442,307);(441,307);(440,307);(439,307);(438,307);(437,307);(436,307);(435,307);(434,307);(433,307);(432,307);(431,307);(430,307);(429,307);(428,307);(427,307);(426,307);(425,307);(424,307);(423,307);(422,307);(421,307);(420,307);(419,307)</t>
-  </si>
-  <si>
-    <t>10</t>
-  </si>
-  <si>
-    <t/>
-  </si>
-  <si>
-    <t xml:space="preserve"> (10)</t>
-  </si>
-  <si>
-    <t>Iron Ore</t>
-  </si>
-  <si>
-    <t>A common metal used for crafting weapons and tools.</t>
-  </si>
-  <si>
-    <t>Color [0.5,0.5,0.5,1]</t>
-  </si>
-  <si>
-    <t>(550,332);(533,461)</t>
-  </si>
-  <si>
-    <t>(550,332);(533,461);(549,333);(548,334);(547,335);(546,336);(545,337);(544,338);(543,339);(542,340);(541,341);(540,342);(539,343);(538,344);(537,345);(536,346);(535,347);(534,348);(533,349);(533,350);(533,351);(533,352);(533,353);(533,354);(533,355);(533,356);(533,357);(533,358);(533,359);(533,360);(533,361);(533,362);(533,363);(533,364);(533,365);(533,366);(533,367);(533,368);(533,369);(533,370);(533,371);(533,372);(533,373);(533,374);(533,375);(533,376);(533,377);(533,378);(533,379);(533,380);(533,381);(533,382);(533,383);(533,384);(533,385);(533,386);(533,387);(533,388);(533,389);(533,390);(533,391);(533,392);(533,393);(533,394);(533,395);(533,396);(533,397);(533,398);(533,399);(533,400);(533,401);(533,402);(533,403);(533,404);(533,405);(533,406);(533,407);(533,408);(533,409);(533,410);(533,411);(533,412);(533,413);(533,414);(533,415);(533,416);(533,417);(533,418);(533,419);(533,420);(533,421);(533,422);(533,423);(533,424);(533,425);(533,426);(533,427);(533,428);(533,429);(533,430);(533,431);(533,432);(533,433);(533,434);(533,435);(533,436);(533,437);(533,438);(533,439);(533,440);(533,441);(533,442);(533,443);(533,444);(533,445);(533,446);(533,447);(533,448);(533,449);(533,450);(533,451);(533,452);(533,453);(533,454);(533,455);(533,456);(533,457);(533,458);(533,459);(533,460);(533,461)</t>
-  </si>
-  <si>
-    <t>14</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (14)</t>
-  </si>
-  <si>
-    <t>(472,582);(365,450)</t>
-  </si>
-  <si>
-    <t>(472,582);(365,450);(471,581);(470,580);(469,579);(468,578);(467,577);(466,576);(465,575);(464,574);(463,573);(462,572);(461,571);(460,570);(459,569);(458,568);(457,567);(456,566);(455,565);(454,564);(453,563);(452,562);(451,561);(450,560);(449,559);(448,558);(447,557);(446,556);(445,555);(444,554);(443,553);(442,552);(441,551);(440,550);(439,549);(438,548);(437,547);(436,546);(435,545);(434,544);(433,543);(432,542);(431,541);(430,540);(429,539);(428,538);(427,537);(426,536);(425,535);(424,534);(423,533);(422,532);(421,531);(420,530);(419,529);(418,528);(417,527);(416,526);(415,525);(414,524);(413,523);(412,522);(411,521);(410,520);(409,519);(408,518);(407,517);(406,516);(405,515);(404,514);(403,513);(402,512);(401,511);(400,510);(399,509);(398,508);(397,507);(396,506);(395,505);(394,504);(393,503);(392,502);(391,501);(390,500);(389,499);(388,498);(387,497);(386,496);(385,495);(384,494);(383,493);(382,492);(381,491);(380,490);(379,489);(378,488);(377,487);(376,486);(375,485);(374,484);(373,483);(372,482);(371,481);(370,480);(369,479);(368,478);(367,477);(366,476);(365,475);(365,474);(365,473);(365,472);(365,471);(365,470);(365,469);(365,468);(365,467);(365,466);(365,465);(365,464);(365,463);(365,462);(365,461);(365,460);(365,459);(365,458);(365,457);(365,456);(365,455);(365,454);(365,453);(365,452);(365,451);(365,450)</t>
-  </si>
-  <si>
-    <t>15</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (15)</t>
-  </si>
-  <si>
-    <t>(523,431);(578,532)</t>
-  </si>
-  <si>
-    <t>(523,431);(578,532);(524,432);(525,433);(526,434);(527,435);(528,436);(529,437);(530,438);(531,439);(532,440);(533,441);(534,442);(535,443);(536,444);(537,445);(538,446);(539,447);(540,448);(541,449);(542,450);(543,451);(544,452);(545,453);(546,454);(547,455);(548,456);(549,457);(550,458);(551,459);(552,460);(553,461);(554,462);(555,463);(556,464);(557,465);(558,466);(559,467);(560,468);(561,469);(562,470);(563,471);(564,472);(565,473);(566,474);(567,475);(568,476);(569,477);(570,478);(571,479);(572,480);(573,481);(574,482);(575,483);(576,484);(577,485);(578,486);(578,487);(578,488);(578,489);(578,490);(578,491);(578,492);(578,493);(578,494);(578,495);(578,496);(578,497);(578,498);(578,499);(578,500);(578,501);(578,502);(578,503);(578,504);(578,505);(578,506);(578,507);(578,508);(578,509);(578,510);(578,511);(578,512);(578,513);(578,514);(578,515);(578,516);(578,517);(578,518);(578,519);(578,520);(578,521);(578,522);(578,523);(578,524);(578,525);(578,526);(578,527);(578,528);(578,529);(578,530);(578,531);(578,532)</t>
-  </si>
-  <si>
-    <t>16</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (16)</t>
-  </si>
-  <si>
-    <t>(439,275);(280,748)</t>
-  </si>
-  <si>
-    <t>(439,275);(280,748);(438,276);(437,277);(436,278);(435,279);(434,280);(433,281);(432,282);(431,283);(430,284);(429,285);(428,286);(427,287);(426,288);(425,289);(424,290);(423,291);(422,292);(421,293);(420,294);(419,295);(418,296);(417,297);(416,298);(415,299);(414,300);(413,301);(412,302);(411,303);(410,304);(409,305);(408,306);(407,307);(406,308);(405,309);(404,310);(403,311);(402,312);(401,313);(400,314);(399,315);(398,316);(397,317);(396,318);(395,319);(394,320);(393,321);(392,322);(391,323);(390,324);(389,325);(388,326);(387,327);(386,328);(385,329);(384,330);(383,331);(382,332);(381,333);(380,334);(379,335);(378,336);(377,337);(376,338);(375,339);(374,340);(373,341);(372,342);(371,343);(370,344);(369,345);(368,346);(367,347);(366,348);(365,349);(364,350);(363,351);(362,352);(361,353);(360,354);(359,355);(358,356);(357,357);(356,358);(355,359);(354,360);(353,361);(352,362);(351,363);(350,364);(349,365);(348,366);(347,367);(346,368);(345,369);(344,370);(343,371);(342,372);(341,373);(340,374);(339,375);(338,376);(337,377);(336,378);(335,379);(334,380);(333,381);(332,382);(331,383);(330,384);(329,385);(328,386);(327,387);(326,388);(325,389);(324,390);(323,391);(322,392);(321,393);(320,394);(319,395);(318,396);(317,397);(316,398);(315,399);(314,400);(313,401);(312,402);(311,403);(310,404);(309,405);(308,406);(307,407);(306,408);(305,409);(304,410);(303,411);(302,412);(301,413);(300,414);(299,415);(298,416);(297,417);(296,418);(295,419);(294,420);(293,421);(292,422);(291,423);(290,424);(289,425);(288,426);(287,427);(286,428);(285,429);(284,430);(283,431);(282,432);(281,433);(280,434);(280,435);(280,436);(280,437);(280,438);(280,439);(280,440);(280,441);(280,442);(280,443);(280,444);(280,445);(280,446);(280,447);(280,448);(280,449);(280,450);(280,451);(280,452);(280,453);(280,454);(280,455);(280,456);(280,457);(280,458);(280,459);(280,460);(280,461);(280,462);(280,463);(280,464);(280,465);(280,466);(280,467);(280,468);(280,469);(280,470);(280,471);(280,472);(280,473);(280,474);(280,475);(280,476);(280,477);(280,478);(280,479);(280,480);(280,481);(280,482);(280,483);(280,484);(280,485);(280,486);(280,487);(280,488);(280,489);(280,490);(280,491);(280,492);(280,493);(280,494);(280,495);(280,496);(280,497);(280,498);(280,499);(280,500);(280,501);(280,502);(280,503);(280,504);(280,505);(280,506);(280,507);(280,508);(280,509);(280,510);(280,511);(280,512);(280,513);(280,514);(280,515);(280,516);(280,517);(280,518);(280,519);(280,520);(280,521);(280,522);(280,523);(280,524);(280,525);(280,526);(280,527);(280,528);(280,529);(280,530);(280,531);(280,532);(280,533);(280,534);(280,535);(280,536);(280,537);(280,538);(280,539);(280,540);(280,541);(280,542);(280,543);(280,544);(280,545);(280,546);(280,547);(280,548);(280,549);(280,550);(280,551);(280,552);(280,553);(280,554);(280,555);(280,556);(280,557);(280,558);(280,559);(280,560);(280,561);(280,562);(280,563);(280,564);(280,565);(280,566);(280,567);(280,568);(280,569);(280,570);(280,571);(280,572);(280,573);(280,574);(280,575);(280,576);(280,577);(280,578);(280,579);(280,580);(280,581);(280,582);(280,583);(280,584);(280,585);(280,586);(280,587);(280,588);(280,589);(280,590);(280,591);(280,592);(280,593);(280,594);(280,595);(280,596);(280,597);(280,598);(280,599);(280,600);(280,601);(280,602);(280,603);(280,604);(280,605);(280,606);(280,607);(280,608);(280,609);(280,610);(280,611);(280,612);(280,613);(280,614);(280,615);(280,616);(280,617);(280,618);(280,619);(280,620);(280,621);(280,622);(280,623);(280,624);(280,625);(280,626);(280,627);(280,628);(280,629);(280,630);(280,631);(280,632);(280,633);(280,634);(280,635);(280,636);(280,637);(280,638);(280,639);(280,640);(280,641);(280,642);(280,643);(280,644);(280,645);(280,646);(280,647);(280,648);(280,649);(280,650);(280,651);(280,652);(280,653);(280,654);(280,655);(280,656);(280,657);(280,658);(280,659);(280,660);(280,661);(280,662);(280,663);(280,664);(280,665);(280,666);(280,667);(280,668);(280,669);(280,670);(280,671);(280,672);(280,673);(280,674);(280,675);(280,676);(280,677);(280,678);(280,679);(280,680);(280,681);(280,682);(280,683);(280,684);(280,685);(280,686);(280,687);(280,688);(280,689);(280,690);(280,691);(280,692);(280,693);(280,694);(280,695);(280,696);(280,697);(280,698);(280,699);(254,622);(567,243)</t>
+    <t xml:space="preserve"> (8)</t>
+  </si>
+  <si>
+    <t>(339,351);(290,576)</t>
+  </si>
+  <si>
+    <t>(339,351);(290,576);(338,352);(337,353);(336,354);(335,355);(334,356);(333,357);(332,358);(331,359);(330,360);(329,361);(328,362);(327,363);(326,364);(325,365);(324,366);(323,367);(322,368);(321,369);(320,370);(319,371);(318,372);(317,373);(316,374);(315,375);(314,376);(313,377);(312,378);(311,379);(310,380);(309,381);(308,382);(307,383);(306,384);(305,385);(304,386);(303,387);(302,388);(301,389);(300,390);(299,391);(298,392);(297,393);(296,394);(295,395);(294,396);(293,397);(292,398);(291,399);(290,400);(290,401);(290,402);(290,403);(290,404);(290,405);(290,406);(290,407);(290,408);(290,409);(290,410);(290,411);(290,412);(290,413);(290,414);(290,415);(290,416);(290,417);(290,418);(290,419);(290,420);(290,421);(290,422);(290,423);(290,424);(290,425);(290,426);(290,427);(290,428);(290,429);(290,430);(290,431);(290,432);(290,433);(290,434);(290,435);(290,436);(290,437);(290,438);(290,439);(290,440);(290,441);(290,442);(290,443);(290,444);(290,445);(290,446);(290,447);(290,448);(290,449);(290,450);(290,451);(290,452);(290,453);(290,454);(290,455);(290,456);(290,457);(290,458);(290,459);(290,460);(290,461);(290,462);(290,463);(290,464);(290,465);(290,466);(290,467);(290,468);(290,469);(290,470);(290,471);(290,472);(290,473);(290,474);(290,475);(290,476);(290,477);(290,478);(290,479);(290,480);(290,481);(290,482);(290,483);(290,484);(290,485);(290,486);(290,487);(290,488);(290,489);(290,490);(290,491);(290,492);(290,493);(290,494);(290,495);(290,496);(290,497);(290,498);(290,499);(290,500);(290,501);(290,502);(290,503);(290,504);(290,505);(290,506);(290,507);(290,508);(290,509);(290,510);(290,511);(290,512);(290,513);(290,514);(290,515);(290,516);(290,517);(290,518);(290,519);(290,520);(290,521);(290,522);(290,523);(290,524);(290,525);(290,526);(290,527);(290,528);(290,529);(290,530);(290,531);(290,532);(290,533);(290,534);(290,535);(290,536);(290,537);(290,538);(290,539);(290,540);(290,541);(290,542);(290,543);(290,544);(290,545);(290,546);(290,547);(290,548);(290,549);(290,550);(290,551);(290,552);(290,553);(290,554);(290,555);(290,556);(290,557);(290,558);(290,559);(290,560);(290,561);(290,562);(290,563);(290,564);(290,565);(290,566);(290,567);(290,568);(290,569);(290,570);(290,571);(290,572);(290,573);(290,574);(290,575);(290,576)</t>
+  </si>
+  <si>
+    <t>9</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (9)</t>
+  </si>
+  <si>
+    <t>(323,569);(573,260)</t>
+  </si>
+  <si>
+    <t>(323,569);(573,260);(324,568);(325,567);(326,566);(327,565);(328,564);(329,563);(330,562);(331,561);(332,560);(333,559);(334,558);(335,557);(336,556);(337,555);(338,554);(339,553);(340,552);(341,551);(342,550);(343,549);(344,548);(345,547);(346,546);(347,545);(348,544);(349,543);(350,542);(351,541);(352,540);(353,539);(354,538);(355,537);(356,536);(357,535);(358,534);(359,533);(360,532);(361,531);(362,530);(363,529);(364,528);(365,527);(366,526);(367,525);(368,524);(369,523);(370,522);(371,521);(372,520);(373,519);(374,518);(375,517);(376,516);(377,515);(378,514);(379,513);(380,512);(381,511);(382,510);(383,509);(384,508);(385,507);(386,506);(387,505);(388,504);(389,503);(390,502);(391,501);(392,500);(393,499);(394,498);(395,497);(396,496);(397,495);(398,494);(399,493);(400,492);(401,491);(402,490);(403,489);(404,488);(405,487);(406,486);(407,485);(408,484);(409,483);(410,482);(411,481);(412,480);(413,479);(414,478);(415,477);(416,476);(417,475);(418,474);(419,473);(420,472);(421,471);(422,470);(423,469);(424,468);(425,467);(426,466);(427,465);(428,464);(429,463);(430,462);(431,461);(432,460);(433,459);(434,458);(435,457);(436,456);(437,455);(438,454);(439,453);(440,452);(441,451);(442,450);(443,449);(444,448);(445,447);(446,446);(447,445);(448,444);(449,443);(450,442);(451,441);(452,440);(453,439);(454,438);(455,437);(456,436);(457,435);(458,434);(459,433);(460,432);(461,431);(462,430);(463,429);(464,428);(465,427);(466,426);(467,425);(468,424);(469,423);(470,422);(471,421);(472,420);(473,419);(474,418);(475,417);(476,416);(477,415);(478,414);(479,413);(480,412);(481,411);(482,410);(483,409);(484,408);(485,407);(486,406);(487,405);(488,404);(489,403);(490,402);(491,401);(492,400);(493,399);(494,398);(495,397);(496,396);(497,395);(498,394);(499,393);(500,392);(501,391);(502,390);(503,389);(504,388);(505,387);(506,386);(507,385);(508,384);(509,383);(510,382);(511,381);(512,380);(513,379);(514,378);(515,377);(516,376);(517,375);(518,374);(519,373);(520,372);(521,371);(522,370);(523,369);(524,368);(525,367);(526,366);(527,365);(528,364);(529,363);(530,362);(531,361);(532,360);(533,359);(534,358);(535,357);(536,356);(537,355);(538,354);(539,353);(540,352);(541,351);(542,350);(543,349);(544,348);(545,347);(546,346);(547,345);(548,344);(549,343);(550,342);(551,341);(552,340);(553,339);(554,338);(555,337);(556,336);(557,335);(558,334);(559,333);(560,332);(561,331);(562,330);(563,329);(564,328);(565,327);(566,326);(567,325);(568,324);(569,323);(570,322);(571,321);(572,320);(573,319);(573,318);(573,317);(573,316);(573,315);(573,314);(573,313);(573,312);(573,311);(573,310);(573,309);(573,308);(573,307);(573,306);(573,305);(573,304);(573,303);(573,302);(573,301);(573,300);(573,299);(573,298);(573,297);(573,296);(573,295);(573,294);(573,293);(573,292);(573,291);(573,290);(573,289);(573,288);(573,287);(573,286);(573,285);(573,284);(573,283);(573,282);(573,281);(573,280);(573,279);(573,278);(573,277);(573,276);(573,275);(573,274);(573,273);(573,272);(573,271);(573,270);(573,269);(573,268);(573,267);(573,266);(573,265);(573,264);(573,263);(573,262);(573,261);(573,260)</t>
   </si>
 </sst>
 </file>
@@ -284,10 +254,10 @@
         <v>14</v>
       </c>
       <c r="F2" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G2" s="0">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="H2" s="0" t="s">
         <v>15</v>
@@ -301,115 +271,115 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="0" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F3" s="0">
+        <v>6</v>
+      </c>
+      <c r="G3" s="0">
+        <v>90</v>
+      </c>
+      <c r="H3" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I3" s="0" t="s">
         <v>18</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="0" t="s">
+      <c r="J3" s="0" t="s">
         <v>19</v>
-      </c>
-      <c r="D3" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E3" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F3" s="0">
-        <v>6</v>
-      </c>
-      <c r="G3" s="0">
-        <v>90</v>
-      </c>
-      <c r="H3" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="0" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" s="0" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="B4" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="D4" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E4" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F4" s="0">
+        <v>6</v>
+      </c>
+      <c r="G4" s="0">
+        <v>90</v>
+      </c>
+      <c r="H4" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="0" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="0" t="s">
+      <c r="J4" s="0" t="s">
         <v>21</v>
-      </c>
-      <c r="F4" s="0">
-        <v>6</v>
-      </c>
-      <c r="G4" s="0">
-        <v>90</v>
-      </c>
-      <c r="H4" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I4" s="0" t="s">
-        <v>27</v>
-      </c>
-      <c r="J4" s="0" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>29</v>
+        <v>10</v>
       </c>
       <c r="B5" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>30</v>
+        <v>12</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="F5" s="0">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G5" s="0">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B6" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F6" s="0">
         <v>6</v>
@@ -418,88 +388,88 @@
         <v>90</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>40</v>
+        <v>13</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>41</v>
+        <v>14</v>
       </c>
       <c r="F7" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G7" s="0">
-        <v>100</v>
+        <v>90</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>43</v>
+        <v>33</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>44</v>
+        <v>34</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>45</v>
+        <v>35</v>
       </c>
       <c r="B8" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>14</v>
+      </c>
+      <c r="F8" s="0">
+        <v>6</v>
+      </c>
+      <c r="G8" s="0">
+        <v>90</v>
+      </c>
+      <c r="H8" s="0" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="J8" s="0" t="s">
         <v>38</v>
-      </c>
-      <c r="C8" s="0" t="s">
-        <v>46</v>
-      </c>
-      <c r="D8" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="E8" s="0" t="s">
-        <v>21</v>
-      </c>
-      <c r="F8" s="0">
-        <v>6</v>
-      </c>
-      <c r="G8" s="0">
-        <v>90</v>
-      </c>
-      <c r="H8" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="I8" s="0" t="s">
-        <v>47</v>
-      </c>
-      <c r="J8" s="0" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>49</v>
+        <v>39</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>50</v>
+        <v>40</v>
       </c>
       <c r="D9" s="0" t="s">
         <v>13</v>
@@ -508,36 +478,36 @@
         <v>14</v>
       </c>
       <c r="F9" s="0">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="G9" s="0">
-        <v>20</v>
+        <v>90</v>
       </c>
       <c r="H9" s="0" t="s">
         <v>15</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="J9" s="0" t="s">
-        <v>52</v>
+        <v>42</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
       <c r="F10" s="0">
         <v>6</v>
@@ -546,13 +516,13 @@
         <v>90</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
working on main screen an game quest
</commit_message>
<xml_diff>
--- a/Mineral.xlsx
+++ b/Mineral.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="595" uniqueCount="595">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="591" uniqueCount="591">
   <si>
     <t>ID</t>
   </si>
@@ -716,10 +716,10 @@
     <t>(345,415);(623,263);(346,414);(347,413);(348,412);(349,411);(350,410);(351,409);(352,408);(353,407);(354,406);(355,405);(356,404);(357,403);(358,402);(359,401);(360,400);(361,399);(362,398);(363,397);(364,396);(365,395);(366,394);(367,393);(368,392);(369,391);(370,390);(371,389);(372,388);(373,387);(374,386);(375,385);(376,384);(377,383);(378,382);(379,381);(380,380);(381,379);(382,378);(383,377);(384,376);(385,375);(386,374);(387,373);(388,372);(389,371);(390,370);(391,369);(392,368);(393,367);(394,366);(395,365);(396,364);(397,363);(398,362);(399,361);(400,360);(401,359);(402,358);(403,357);(404,356);(405,355);(406,354);(407,353);(408,352);(409,351);(410,350);(411,349);(412,348);(413,347);(414,346);(415,345);(416,344);(417,343);(418,342);(419,341);(420,340);(421,339);(422,338);(423,337);(424,336);(425,335);(426,334);(427,333);(428,332);(429,331);(430,330);(431,329);(432,328);(433,327);(434,326);(435,325);(436,324);(437,323);(438,322);(439,321);(440,320);(441,319);(442,318);(443,317);(444,316);(445,315);(446,314);(447,313);(448,312);(449,311);(450,310);(451,309);(452,308);(453,307);(454,306);(455,305);(456,304);(457,303);(458,302);(459,301);(460,300);(461,299);(462,298);(463,297);(464,296);(465,295);(466,294);(467,293);(468,292);(469,291);(470,290);(471,289);(472,288);(473,287);(474,286);(475,285);(476,284);(477,283);(478,282);(479,281);(480,280);(481,279);(482,278);(483,277);(484,276);(485,275);(486,274);(487,273);(488,272);(489,271);(490,270);(491,269);(492,268);(493,267);(494,266);(495,265);(496,264);(497,263);(498,263);(499,263);(500,263);(501,263);(502,263);(503,263);(504,263);(505,263);(506,263);(507,263);(508,263);(509,263);(510,263);(511,263);(512,263);(513,263);(514,263);(515,263);(516,263);(517,263);(518,263);(519,263);(520,263);(521,263);(522,263);(523,263);(524,263);(525,263);(526,263);(527,263);(528,263);(529,263);(530,263);(531,263);(532,263);(533,263);(534,263);(535,263);(536,263);(537,263);(538,263);(539,263);(540,263);(541,263);(542,263);(543,263);(544,263);(545,263);(546,263);(547,263);(548,263);(549,263);(550,263);(551,263);(552,263);(553,263);(554,263);(555,263);(556,263);(557,263);(558,263);(559,263);(560,263);(561,263);(562,263);(563,263);(564,263);(565,263);(566,263);(567,263);(568,263);(569,263);(570,263);(571,263);(572,263);(573,263);(574,263);(575,263);(576,263);(577,263);(578,263);(579,263);(580,263);(581,263);(582,263);(583,263);(584,263);(585,263);(586,263);(587,263);(588,263);(589,263);(590,263);(591,263);(592,263);(593,263);(594,263);(595,263);(596,263);(597,263);(598,263);(599,263);(600,263);(601,263);(602,263);(603,263);(604,263);(605,263);(606,263);(607,263);(608,263);(609,263);(610,263);(611,263);(612,263);(613,263);(614,263);(615,263);(616,263);(617,263);(618,263);(619,263);(620,263);(621,263);(622,263);(623,263)</t>
   </si>
   <si>
-    <t>49</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (49)</t>
+    <t>50</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> (50)</t>
   </si>
   <si>
     <t>Adamantium</t>
@@ -729,18 +729,6 @@
   </si>
   <si>
     <t>Color [0.6627451,0.6627451,0.6627451,1]</t>
-  </si>
-  <si>
-    <t>(727,412);(247,698)</t>
-  </si>
-  <si>
-    <t>(727,412);(247,698);(726,413);(725,414);(724,415);(723,416);(722,417);(721,418);(720,419);(719,420);(718,421);(717,422);(716,423);(715,424);(714,425);(713,426);(712,427);(711,428);(710,429);(709,430);(708,431);(707,432);(706,433);(705,434);(704,435);(703,436);(702,437);(701,438);(700,439);(699,440);(698,441);(697,442);(696,443);(695,444);(694,445);(693,446);(692,447);(691,448);(690,449);(689,450);(688,451);(687,452);(686,453);(685,454);(684,455);(683,456);(682,457);(681,458);(680,459);(679,460);(678,461);(677,462);(676,463);(675,464);(674,465);(673,466);(672,467);(671,468);(670,469);(669,470);(668,471);(667,472);(666,473);(665,474);(664,475);(663,476);(662,477);(661,478);(660,479);(659,480);(658,481);(657,482);(656,483);(655,484);(654,485);(653,486);(652,487);(651,488);(650,489);(649,490);(648,491);(647,492);(646,493);(645,494);(644,495);(643,496);(642,497);(641,498);(640,499);(639,500);(638,501);(637,502);(636,503);(635,504);(634,505);(633,506);(632,507);(631,508);(630,509);(629,510);(628,511);(627,512);(626,513);(625,514);(624,515);(623,516);(622,517);(621,518);(620,519);(619,520);(618,521);(617,522);(616,523);(615,524);(614,525);(613,526);(612,527);(611,528);(610,529);(609,530);(608,531);(607,532);(606,533);(605,534);(604,535);(603,536);(602,537);(601,538);(600,539);(599,540);(598,541);(597,542);(596,543);(595,544);(594,545);(593,546);(592,547);(591,548);(590,549);(589,550);(588,551);(587,552);(586,553);(585,554);(584,555);(583,556);(582,557);(581,558);(580,559);(579,560);(578,561);(577,562);(576,563);(575,564);(574,565);(573,566);(572,567);(571,568);(570,569);(569,570);(568,571);(567,572);(566,573);(565,574);(564,575);(563,576);(562,577);(561,578);(560,579);(559,580);(558,581);(557,582);(556,583);(555,584);(554,585);(553,586);(552,587);(551,588);(550,589);(549,590);(548,591);(547,592);(546,593);(545,594);(544,595);(543,596);(542,597);(541,598);(540,599);(539,600);(538,601);(537,602);(536,603);(535,604);(534,605);(533,606);(532,607);(531,608);(530,609);(529,610);(528,611);(527,612);(526,613);(525,614);(524,615);(523,616);(522,617);(521,618);(520,619);(519,620);(518,621);(517,622);(516,623);(515,624);(514,625);(513,626);(512,627);(511,628);(510,629);(509,630);(508,631);(507,632);(506,633);(505,634);(504,635);(503,636);(502,637);(501,638);(500,639);(499,640);(498,641);(497,642);(496,643);(495,644);(494,645);(493,646);(492,647);(491,648);(490,649);(489,650);(488,651);(487,652);(486,653);(485,654);(484,655);(483,656);(482,657);(481,658);(480,659);(479,660);(478,661);(477,662);(476,663);(475,664);(474,665);(473,666);(472,667);(471,668);(470,669);(469,670);(468,671);(467,672);(466,673);(465,674);(464,675);(463,676);(462,677);(461,678);(460,679);(459,680);(458,681);(457,682);(456,683);(455,684);(454,685);(453,686);(452,687);(451,688);(450,689);(449,690);(448,691);(447,692);(446,693);(445,694);(444,695);(443,696);(442,697);(441,698);(440,698);(439,698);(438,698);(437,698);(436,698);(435,698);(434,698);(433,698);(432,698);(431,698);(430,698);(429,698);(428,698);(427,698);(426,698);(425,698);(424,698);(423,698);(422,698);(421,698);(420,698);(419,698);(418,698);(417,698);(416,698);(415,698);(414,698);(413,698);(412,698);(411,698);(410,698);(409,698);(408,698);(407,698);(406,698);(405,698);(404,698);(403,698);(402,698);(401,698);(400,698);(399,698);(398,698);(397,698);(396,698);(395,698);(394,698);(393,698);(392,698);(391,698);(390,698);(389,698);(388,698);(387,698);(386,698);(385,698);(384,698);(383,698);(382,698);(381,698);(380,698);(379,698);(378,698);(377,698);(376,698);(375,698);(374,698);(373,698);(372,698);(371,698);(370,698);(369,698);(368,698);(367,698);(366,698);(365,698);(364,698);(363,698);(362,698);(361,698);(360,698);(359,698);(358,698);(357,698);(356,698);(355,698);(354,698);(353,698);(352,698);(351,698);(350,698);(349,698);(348,698);(347,698);(346,698);(345,698);(344,698);(343,698);(342,698);(341,698);(340,698);(339,698);(338,698);(337,698);(336,698);(335,698);(334,698);(333,698);(332,698);(331,698);(330,698);(329,698);(328,698);(327,698);(326,698);(325,698);(324,698);(323,698);(322,698);(321,698);(320,698);(319,698);(318,698);(317,698);(316,698);(315,698);(314,698);(313,698);(312,698);(311,698);(310,698);(309,698);(308,698);(307,698);(306,698);(305,698);(304,698);(303,698);(302,698);(301,698);(300,698);(299,698);(298,698);(297,698);(296,698);(295,698);(294,698);(293,698);(292,698);(291,698);(290,698);(289,698);(288,698);(287,698);(286,698);(285,698);(284,698);(283,698);(282,698);(281,698);(280,698);(279,698);(278,698);(277,698);(276,698);(275,698);(274,698);(273,698);(272,698);(271,698);(270,698);(269,698);(268,698);(267,698);(266,698);(265,698);(264,698);(263,698);(262,698);(261,698);(260,698);(259,698);(258,698);(257,698);(256,698);(255,698);(254,698);(253,698);(252,698);(251,698);(250,698);(249,698);(248,698);(247,698)</t>
-  </si>
-  <si>
-    <t>50</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> (50)</t>
   </si>
   <si>
     <t>(565,361);(479,712)</t>
@@ -1843,7 +1831,7 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr codeName=""/>
-  <dimension ref="A1:J128"/>
+  <dimension ref="A1:J127"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -3396,42 +3384,42 @@
         <v>250</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>236</v>
+        <v>251</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>237</v>
+        <v>252</v>
       </c>
       <c r="F49" s="0">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="G49" s="0">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>238</v>
+        <v>253</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>251</v>
+        <v>254</v>
       </c>
       <c r="J49" s="0" t="s">
-        <v>252</v>
+        <v>255</v>
       </c>
     </row>
     <row r="50">
       <c r="A50" s="0" t="s">
-        <v>253</v>
+        <v>256</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>254</v>
+        <v>257</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F50" s="0">
         <v>6</v>
@@ -3440,7 +3428,7 @@
         <v>40</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I50" s="0" t="s">
         <v>258</v>
@@ -3460,10 +3448,10 @@
         <v>261</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F51" s="0">
         <v>6</v>
@@ -3472,7 +3460,7 @@
         <v>40</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I51" s="0" t="s">
         <v>262</v>
@@ -3492,10 +3480,10 @@
         <v>265</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F52" s="0">
         <v>6</v>
@@ -3504,7 +3492,7 @@
         <v>40</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I52" s="0" t="s">
         <v>266</v>
@@ -3524,10 +3512,10 @@
         <v>269</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F53" s="0">
         <v>6</v>
@@ -3536,7 +3524,7 @@
         <v>40</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I53" s="0" t="s">
         <v>270</v>
@@ -3556,10 +3544,10 @@
         <v>273</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F54" s="0">
         <v>6</v>
@@ -3568,7 +3556,7 @@
         <v>40</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I54" s="0" t="s">
         <v>274</v>
@@ -3588,10 +3576,10 @@
         <v>277</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F55" s="0">
         <v>6</v>
@@ -3600,7 +3588,7 @@
         <v>40</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I55" s="0" t="s">
         <v>278</v>
@@ -3620,10 +3608,10 @@
         <v>281</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="F56" s="0">
         <v>6</v>
@@ -3632,7 +3620,7 @@
         <v>40</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="I56" s="0" t="s">
         <v>282</v>
@@ -3652,19 +3640,19 @@
         <v>285</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>255</v>
+        <v>236</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>256</v>
+        <v>237</v>
       </c>
       <c r="F57" s="0">
-        <v>6</v>
+        <v>10</v>
       </c>
       <c r="G57" s="0">
-        <v>40</v>
+        <v>10</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>257</v>
+        <v>238</v>
       </c>
       <c r="I57" s="0" t="s">
         <v>286</v>
@@ -3972,42 +3960,42 @@
         <v>325</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>236</v>
+        <v>326</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>237</v>
+        <v>327</v>
       </c>
       <c r="F67" s="0">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="G67" s="0">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>238</v>
+        <v>328</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="J67" s="0" t="s">
-        <v>327</v>
+        <v>330</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" s="0" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="B68" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>329</v>
+        <v>332</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F68" s="0">
         <v>7</v>
@@ -4016,7 +4004,7 @@
         <v>20</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I68" s="0" t="s">
         <v>333</v>
@@ -4036,10 +4024,10 @@
         <v>336</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F69" s="0">
         <v>7</v>
@@ -4048,7 +4036,7 @@
         <v>20</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I69" s="0" t="s">
         <v>337</v>
@@ -4068,10 +4056,10 @@
         <v>340</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="F70" s="0">
         <v>7</v>
@@ -4080,7 +4068,7 @@
         <v>20</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="I70" s="0" t="s">
         <v>341</v>
@@ -4100,42 +4088,42 @@
         <v>344</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>330</v>
+        <v>345</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>331</v>
+        <v>346</v>
       </c>
       <c r="F71" s="0">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G71" s="0">
         <v>20</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>332</v>
+        <v>347</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>345</v>
+        <v>348</v>
       </c>
       <c r="J71" s="0" t="s">
-        <v>346</v>
+        <v>349</v>
       </c>
     </row>
     <row r="72">
       <c r="A72" s="0" t="s">
-        <v>347</v>
+        <v>350</v>
       </c>
       <c r="B72" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C72" s="0" t="s">
-        <v>348</v>
+        <v>351</v>
       </c>
       <c r="D72" s="0" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E72" s="0" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F72" s="0">
         <v>4</v>
@@ -4144,7 +4132,7 @@
         <v>20</v>
       </c>
       <c r="H72" s="0" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="I72" s="0" t="s">
         <v>352</v>
@@ -4164,10 +4152,10 @@
         <v>355</v>
       </c>
       <c r="D73" s="0" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="E73" s="0" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="F73" s="0">
         <v>4</v>
@@ -4176,7 +4164,7 @@
         <v>20</v>
       </c>
       <c r="H73" s="0" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="I73" s="0" t="s">
         <v>356</v>
@@ -4196,170 +4184,170 @@
         <v>359</v>
       </c>
       <c r="D74" s="0" t="s">
-        <v>349</v>
+        <v>360</v>
       </c>
       <c r="E74" s="0" t="s">
-        <v>350</v>
+        <v>361</v>
       </c>
       <c r="F74" s="0">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="G74" s="0">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="H74" s="0" t="s">
-        <v>351</v>
+        <v>362</v>
       </c>
       <c r="I74" s="0" t="s">
-        <v>360</v>
+        <v>363</v>
       </c>
       <c r="J74" s="0" t="s">
-        <v>361</v>
+        <v>364</v>
       </c>
     </row>
     <row r="75">
       <c r="A75" s="0" t="s">
-        <v>362</v>
+        <v>365</v>
       </c>
       <c r="B75" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C75" s="0" t="s">
-        <v>363</v>
+        <v>366</v>
       </c>
       <c r="D75" s="0" t="s">
-        <v>364</v>
+        <v>367</v>
       </c>
       <c r="E75" s="0" t="s">
-        <v>365</v>
+        <v>127</v>
       </c>
       <c r="F75" s="0">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G75" s="0">
-        <v>60</v>
+        <v>25</v>
       </c>
       <c r="H75" s="0" t="s">
-        <v>366</v>
+        <v>368</v>
       </c>
       <c r="I75" s="0" t="s">
-        <v>367</v>
+        <v>369</v>
       </c>
       <c r="J75" s="0" t="s">
-        <v>368</v>
+        <v>370</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" s="0" t="s">
-        <v>369</v>
+        <v>371</v>
       </c>
       <c r="B76" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C76" s="0" t="s">
-        <v>370</v>
+        <v>372</v>
       </c>
       <c r="D76" s="0" t="s">
-        <v>371</v>
+        <v>373</v>
       </c>
       <c r="E76" s="0" t="s">
-        <v>127</v>
+        <v>374</v>
       </c>
       <c r="F76" s="0">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="G76" s="0">
-        <v>25</v>
+        <v>10</v>
       </c>
       <c r="H76" s="0" t="s">
-        <v>372</v>
+        <v>375</v>
       </c>
       <c r="I76" s="0" t="s">
-        <v>373</v>
+        <v>376</v>
       </c>
       <c r="J76" s="0" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
     </row>
     <row r="77">
       <c r="A77" s="0" t="s">
-        <v>375</v>
+        <v>378</v>
       </c>
       <c r="B77" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C77" s="0" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="D77" s="0" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="E77" s="0" t="s">
-        <v>378</v>
+        <v>79</v>
       </c>
       <c r="F77" s="0">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G77" s="0">
-        <v>10</v>
+        <v>15</v>
       </c>
       <c r="H77" s="0" t="s">
-        <v>379</v>
+        <v>80</v>
       </c>
       <c r="I77" s="0" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="J77" s="0" t="s">
-        <v>381</v>
+        <v>382</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" s="0" t="s">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="B78" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C78" s="0" t="s">
-        <v>383</v>
+        <v>384</v>
       </c>
       <c r="D78" s="0" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E78" s="0" t="s">
-        <v>79</v>
+        <v>386</v>
       </c>
       <c r="F78" s="0">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G78" s="0">
-        <v>15</v>
+        <v>60</v>
       </c>
       <c r="H78" s="0" t="s">
-        <v>80</v>
+        <v>387</v>
       </c>
       <c r="I78" s="0" t="s">
-        <v>385</v>
+        <v>388</v>
       </c>
       <c r="J78" s="0" t="s">
-        <v>386</v>
+        <v>389</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" s="0" t="s">
-        <v>387</v>
+        <v>390</v>
       </c>
       <c r="B79" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C79" s="0" t="s">
-        <v>388</v>
+        <v>391</v>
       </c>
       <c r="D79" s="0" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E79" s="0" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="F79" s="0">
         <v>5</v>
@@ -4368,7 +4356,7 @@
         <v>60</v>
       </c>
       <c r="H79" s="0" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="I79" s="0" t="s">
         <v>392</v>
@@ -4388,10 +4376,10 @@
         <v>395</v>
       </c>
       <c r="D80" s="0" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E80" s="0" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="F80" s="0">
         <v>5</v>
@@ -4400,7 +4388,7 @@
         <v>60</v>
       </c>
       <c r="H80" s="0" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="I80" s="0" t="s">
         <v>396</v>
@@ -4420,10 +4408,10 @@
         <v>399</v>
       </c>
       <c r="D81" s="0" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E81" s="0" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="F81" s="0">
         <v>5</v>
@@ -4432,7 +4420,7 @@
         <v>60</v>
       </c>
       <c r="H81" s="0" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="I81" s="0" t="s">
         <v>400</v>
@@ -4452,10 +4440,10 @@
         <v>403</v>
       </c>
       <c r="D82" s="0" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E82" s="0" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="F82" s="0">
         <v>5</v>
@@ -4464,7 +4452,7 @@
         <v>60</v>
       </c>
       <c r="H82" s="0" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="I82" s="0" t="s">
         <v>404</v>
@@ -4484,10 +4472,10 @@
         <v>407</v>
       </c>
       <c r="D83" s="0" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E83" s="0" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="F83" s="0">
         <v>5</v>
@@ -4496,7 +4484,7 @@
         <v>60</v>
       </c>
       <c r="H83" s="0" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="I83" s="0" t="s">
         <v>408</v>
@@ -4516,10 +4504,10 @@
         <v>411</v>
       </c>
       <c r="D84" s="0" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E84" s="0" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="F84" s="0">
         <v>5</v>
@@ -4528,7 +4516,7 @@
         <v>60</v>
       </c>
       <c r="H84" s="0" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="I84" s="0" t="s">
         <v>412</v>
@@ -4548,42 +4536,42 @@
         <v>415</v>
       </c>
       <c r="D85" s="0" t="s">
-        <v>389</v>
+        <v>416</v>
       </c>
       <c r="E85" s="0" t="s">
-        <v>390</v>
+        <v>417</v>
       </c>
       <c r="F85" s="0">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G85" s="0">
-        <v>60</v>
+        <v>200</v>
       </c>
       <c r="H85" s="0" t="s">
-        <v>391</v>
+        <v>418</v>
       </c>
       <c r="I85" s="0" t="s">
-        <v>416</v>
+        <v>419</v>
       </c>
       <c r="J85" s="0" t="s">
-        <v>417</v>
+        <v>420</v>
       </c>
     </row>
     <row r="86">
       <c r="A86" s="0" t="s">
-        <v>418</v>
+        <v>421</v>
       </c>
       <c r="B86" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C86" s="0" t="s">
-        <v>419</v>
+        <v>422</v>
       </c>
       <c r="D86" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E86" s="0" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F86" s="0">
         <v>2</v>
@@ -4592,7 +4580,7 @@
         <v>200</v>
       </c>
       <c r="H86" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I86" s="0" t="s">
         <v>423</v>
@@ -4612,10 +4600,10 @@
         <v>426</v>
       </c>
       <c r="D87" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E87" s="0" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F87" s="0">
         <v>2</v>
@@ -4624,7 +4612,7 @@
         <v>200</v>
       </c>
       <c r="H87" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I87" s="0" t="s">
         <v>427</v>
@@ -4644,10 +4632,10 @@
         <v>430</v>
       </c>
       <c r="D88" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E88" s="0" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F88" s="0">
         <v>2</v>
@@ -4656,7 +4644,7 @@
         <v>200</v>
       </c>
       <c r="H88" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I88" s="0" t="s">
         <v>431</v>
@@ -4676,10 +4664,10 @@
         <v>434</v>
       </c>
       <c r="D89" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E89" s="0" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F89" s="0">
         <v>2</v>
@@ -4688,7 +4676,7 @@
         <v>200</v>
       </c>
       <c r="H89" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I89" s="0" t="s">
         <v>435</v>
@@ -4708,10 +4696,10 @@
         <v>438</v>
       </c>
       <c r="D90" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E90" s="0" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F90" s="0">
         <v>2</v>
@@ -4720,7 +4708,7 @@
         <v>200</v>
       </c>
       <c r="H90" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I90" s="0" t="s">
         <v>439</v>
@@ -4740,10 +4728,10 @@
         <v>442</v>
       </c>
       <c r="D91" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E91" s="0" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F91" s="0">
         <v>2</v>
@@ -4752,7 +4740,7 @@
         <v>200</v>
       </c>
       <c r="H91" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I91" s="0" t="s">
         <v>443</v>
@@ -4772,10 +4760,10 @@
         <v>446</v>
       </c>
       <c r="D92" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E92" s="0" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F92" s="0">
         <v>2</v>
@@ -4784,7 +4772,7 @@
         <v>200</v>
       </c>
       <c r="H92" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I92" s="0" t="s">
         <v>447</v>
@@ -4804,10 +4792,10 @@
         <v>450</v>
       </c>
       <c r="D93" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E93" s="0" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F93" s="0">
         <v>2</v>
@@ -4816,30 +4804,30 @@
         <v>200</v>
       </c>
       <c r="H93" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I93" s="0" t="s">
         <v>451</v>
       </c>
       <c r="J93" s="0" t="s">
-        <v>452</v>
+        <v>451</v>
       </c>
     </row>
     <row r="94">
       <c r="A94" s="0" t="s">
+        <v>452</v>
+      </c>
+      <c r="B94" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C94" s="0" t="s">
         <v>453</v>
       </c>
-      <c r="B94" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C94" s="0" t="s">
-        <v>454</v>
-      </c>
       <c r="D94" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E94" s="0" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F94" s="0">
         <v>2</v>
@@ -4848,10 +4836,10 @@
         <v>200</v>
       </c>
       <c r="H94" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I94" s="0" t="s">
-        <v>455</v>
+        <v>454</v>
       </c>
       <c r="J94" s="0" t="s">
         <v>455</v>
@@ -4868,10 +4856,10 @@
         <v>457</v>
       </c>
       <c r="D95" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E95" s="0" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F95" s="0">
         <v>2</v>
@@ -4880,7 +4868,7 @@
         <v>200</v>
       </c>
       <c r="H95" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I95" s="0" t="s">
         <v>458</v>
@@ -4900,10 +4888,10 @@
         <v>461</v>
       </c>
       <c r="D96" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E96" s="0" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F96" s="0">
         <v>2</v>
@@ -4912,7 +4900,7 @@
         <v>200</v>
       </c>
       <c r="H96" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I96" s="0" t="s">
         <v>462</v>
@@ -4932,10 +4920,10 @@
         <v>465</v>
       </c>
       <c r="D97" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E97" s="0" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F97" s="0">
         <v>2</v>
@@ -4944,7 +4932,7 @@
         <v>200</v>
       </c>
       <c r="H97" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I97" s="0" t="s">
         <v>466</v>
@@ -4964,10 +4952,10 @@
         <v>469</v>
       </c>
       <c r="D98" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E98" s="0" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F98" s="0">
         <v>2</v>
@@ -4976,7 +4964,7 @@
         <v>200</v>
       </c>
       <c r="H98" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I98" s="0" t="s">
         <v>470</v>
@@ -4996,10 +4984,10 @@
         <v>473</v>
       </c>
       <c r="D99" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E99" s="0" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F99" s="0">
         <v>2</v>
@@ -5008,7 +4996,7 @@
         <v>200</v>
       </c>
       <c r="H99" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I99" s="0" t="s">
         <v>474</v>
@@ -5028,10 +5016,10 @@
         <v>477</v>
       </c>
       <c r="D100" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E100" s="0" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F100" s="0">
         <v>2</v>
@@ -5040,7 +5028,7 @@
         <v>200</v>
       </c>
       <c r="H100" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I100" s="0" t="s">
         <v>478</v>
@@ -5060,10 +5048,10 @@
         <v>481</v>
       </c>
       <c r="D101" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E101" s="0" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F101" s="0">
         <v>2</v>
@@ -5072,7 +5060,7 @@
         <v>200</v>
       </c>
       <c r="H101" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I101" s="0" t="s">
         <v>482</v>
@@ -5092,10 +5080,10 @@
         <v>485</v>
       </c>
       <c r="D102" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E102" s="0" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F102" s="0">
         <v>2</v>
@@ -5104,7 +5092,7 @@
         <v>200</v>
       </c>
       <c r="H102" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I102" s="0" t="s">
         <v>486</v>
@@ -5124,10 +5112,10 @@
         <v>489</v>
       </c>
       <c r="D103" s="0" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E103" s="0" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="F103" s="0">
         <v>2</v>
@@ -5136,7 +5124,7 @@
         <v>200</v>
       </c>
       <c r="H103" s="0" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="I103" s="0" t="s">
         <v>490</v>
@@ -5156,19 +5144,19 @@
         <v>493</v>
       </c>
       <c r="D104" s="0" t="s">
-        <v>420</v>
+        <v>71</v>
       </c>
       <c r="E104" s="0" t="s">
-        <v>421</v>
+        <v>72</v>
       </c>
       <c r="F104" s="0">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G104" s="0">
-        <v>200</v>
+        <v>25</v>
       </c>
       <c r="H104" s="0" t="s">
-        <v>422</v>
+        <v>73</v>
       </c>
       <c r="I104" s="0" t="s">
         <v>494</v>
@@ -5252,19 +5240,19 @@
         <v>505</v>
       </c>
       <c r="D107" s="0" t="s">
-        <v>71</v>
+        <v>380</v>
       </c>
       <c r="E107" s="0" t="s">
-        <v>72</v>
+        <v>79</v>
       </c>
       <c r="F107" s="0">
         <v>7</v>
       </c>
       <c r="G107" s="0">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="H107" s="0" t="s">
-        <v>73</v>
+        <v>80</v>
       </c>
       <c r="I107" s="0" t="s">
         <v>506</v>
@@ -5284,7 +5272,7 @@
         <v>509</v>
       </c>
       <c r="D108" s="0" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="E108" s="0" t="s">
         <v>79</v>
@@ -5316,7 +5304,7 @@
         <v>513</v>
       </c>
       <c r="D109" s="0" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="E109" s="0" t="s">
         <v>79</v>
@@ -5348,7 +5336,7 @@
         <v>517</v>
       </c>
       <c r="D110" s="0" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="E110" s="0" t="s">
         <v>79</v>
@@ -5380,42 +5368,42 @@
         <v>521</v>
       </c>
       <c r="D111" s="0" t="s">
-        <v>384</v>
+        <v>522</v>
       </c>
       <c r="E111" s="0" t="s">
-        <v>79</v>
+        <v>523</v>
       </c>
       <c r="F111" s="0">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="G111" s="0">
-        <v>15</v>
+        <v>50</v>
       </c>
       <c r="H111" s="0" t="s">
-        <v>80</v>
+        <v>524</v>
       </c>
       <c r="I111" s="0" t="s">
-        <v>522</v>
+        <v>525</v>
       </c>
       <c r="J111" s="0" t="s">
-        <v>523</v>
+        <v>526</v>
       </c>
     </row>
     <row r="112">
       <c r="A112" s="0" t="s">
-        <v>524</v>
+        <v>527</v>
       </c>
       <c r="B112" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C112" s="0" t="s">
-        <v>525</v>
+        <v>528</v>
       </c>
       <c r="D112" s="0" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E112" s="0" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="F112" s="0">
         <v>6</v>
@@ -5424,7 +5412,7 @@
         <v>50</v>
       </c>
       <c r="H112" s="0" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="I112" s="0" t="s">
         <v>529</v>
@@ -5444,10 +5432,10 @@
         <v>532</v>
       </c>
       <c r="D113" s="0" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E113" s="0" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="F113" s="0">
         <v>6</v>
@@ -5456,7 +5444,7 @@
         <v>50</v>
       </c>
       <c r="H113" s="0" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="I113" s="0" t="s">
         <v>533</v>
@@ -5476,10 +5464,10 @@
         <v>536</v>
       </c>
       <c r="D114" s="0" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E114" s="0" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="F114" s="0">
         <v>6</v>
@@ -5488,7 +5476,7 @@
         <v>50</v>
       </c>
       <c r="H114" s="0" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="I114" s="0" t="s">
         <v>537</v>
@@ -5508,10 +5496,10 @@
         <v>540</v>
       </c>
       <c r="D115" s="0" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E115" s="0" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="F115" s="0">
         <v>6</v>
@@ -5520,7 +5508,7 @@
         <v>50</v>
       </c>
       <c r="H115" s="0" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="I115" s="0" t="s">
         <v>541</v>
@@ -5540,10 +5528,10 @@
         <v>544</v>
       </c>
       <c r="D116" s="0" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E116" s="0" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="F116" s="0">
         <v>6</v>
@@ -5552,7 +5540,7 @@
         <v>50</v>
       </c>
       <c r="H116" s="0" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="I116" s="0" t="s">
         <v>545</v>
@@ -5572,10 +5560,10 @@
         <v>548</v>
       </c>
       <c r="D117" s="0" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E117" s="0" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="F117" s="0">
         <v>6</v>
@@ -5584,7 +5572,7 @@
         <v>50</v>
       </c>
       <c r="H117" s="0" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="I117" s="0" t="s">
         <v>549</v>
@@ -5604,10 +5592,10 @@
         <v>552</v>
       </c>
       <c r="D118" s="0" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E118" s="0" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="F118" s="0">
         <v>6</v>
@@ -5616,7 +5604,7 @@
         <v>50</v>
       </c>
       <c r="H118" s="0" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="I118" s="0" t="s">
         <v>553</v>
@@ -5636,10 +5624,10 @@
         <v>556</v>
       </c>
       <c r="D119" s="0" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E119" s="0" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="F119" s="0">
         <v>6</v>
@@ -5648,7 +5636,7 @@
         <v>50</v>
       </c>
       <c r="H119" s="0" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="I119" s="0" t="s">
         <v>557</v>
@@ -5668,10 +5656,10 @@
         <v>560</v>
       </c>
       <c r="D120" s="0" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E120" s="0" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="F120" s="0">
         <v>6</v>
@@ -5680,7 +5668,7 @@
         <v>50</v>
       </c>
       <c r="H120" s="0" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="I120" s="0" t="s">
         <v>561</v>
@@ -5700,10 +5688,10 @@
         <v>564</v>
       </c>
       <c r="D121" s="0" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E121" s="0" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="F121" s="0">
         <v>6</v>
@@ -5712,7 +5700,7 @@
         <v>50</v>
       </c>
       <c r="H121" s="0" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="I121" s="0" t="s">
         <v>565</v>
@@ -5732,10 +5720,10 @@
         <v>568</v>
       </c>
       <c r="D122" s="0" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E122" s="0" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="F122" s="0">
         <v>6</v>
@@ -5744,7 +5732,7 @@
         <v>50</v>
       </c>
       <c r="H122" s="0" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="I122" s="0" t="s">
         <v>569</v>
@@ -5764,10 +5752,10 @@
         <v>572</v>
       </c>
       <c r="D123" s="0" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="E123" s="0" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="F123" s="0">
         <v>6</v>
@@ -5776,7 +5764,7 @@
         <v>50</v>
       </c>
       <c r="H123" s="0" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="I123" s="0" t="s">
         <v>573</v>
@@ -5796,19 +5784,19 @@
         <v>576</v>
       </c>
       <c r="D124" s="0" t="s">
-        <v>526</v>
+        <v>13</v>
       </c>
       <c r="E124" s="0" t="s">
-        <v>527</v>
+        <v>14</v>
       </c>
       <c r="F124" s="0">
         <v>6</v>
       </c>
       <c r="G124" s="0">
-        <v>50</v>
+        <v>90</v>
       </c>
       <c r="H124" s="0" t="s">
-        <v>528</v>
+        <v>15</v>
       </c>
       <c r="I124" s="0" t="s">
         <v>577</v>
@@ -5911,38 +5899,6 @@
       </c>
       <c r="J127" s="0" t="s">
         <v>590</v>
-      </c>
-    </row>
-    <row r="128">
-      <c r="A128" s="0" t="s">
-        <v>591</v>
-      </c>
-      <c r="B128" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C128" s="0" t="s">
-        <v>592</v>
-      </c>
-      <c r="D128" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E128" s="0" t="s">
-        <v>14</v>
-      </c>
-      <c r="F128" s="0">
-        <v>6</v>
-      </c>
-      <c r="G128" s="0">
-        <v>90</v>
-      </c>
-      <c r="H128" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="I128" s="0" t="s">
-        <v>593</v>
-      </c>
-      <c r="J128" s="0" t="s">
-        <v>594</v>
       </c>
     </row>
   </sheetData>

</xml_diff>